<commit_message>
Added JDBC methods to get data from the database to Java, addeded in the employee information frame with card layout, added the notes structure(model) and the GUI to create the notes. Started on calender and dashboard pages.
</commit_message>
<xml_diff>
--- a/Development Timelines/GanttChart_Iteration3.xlsx
+++ b/Development Timelines/GanttChart_Iteration3.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED37150A-1419-4EAA-8870-175E8FE986D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A6F2AF-B948-4B49-A9BC-A3D3931820E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5868" yWindow="-108" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -768,6 +768,14 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -780,14 +788,6 @@
     <xf numFmtId="166" fontId="6" fillId="0" borderId="3" xfId="8">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Comma" xfId="3" builtinId="3" customBuiltin="1"/>
@@ -1445,9 +1445,9 @@
   </sheetPr>
   <dimension ref="A1:GU49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="29" zoomScaleNormal="40" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1573,10 +1573,10 @@
       <c r="C3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="44">
+      <c r="D3" s="48">
         <v>44844</v>
       </c>
-      <c r="E3" s="44"/>
+      <c r="E3" s="48"/>
     </row>
     <row r="4" spans="1:203" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
@@ -1588,286 +1588,286 @@
       <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="H4" s="41">
+      <c r="H4" s="45">
         <f>H5</f>
         <v>44844</v>
       </c>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="41">
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="45">
         <f>O5</f>
         <v>44851</v>
       </c>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="42"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="42"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="41">
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="46"/>
+      <c r="T4" s="46"/>
+      <c r="U4" s="47"/>
+      <c r="V4" s="45">
         <f>V5</f>
         <v>44858</v>
       </c>
-      <c r="W4" s="42"/>
-      <c r="X4" s="42"/>
-      <c r="Y4" s="42"/>
-      <c r="Z4" s="42"/>
-      <c r="AA4" s="42"/>
-      <c r="AB4" s="43"/>
-      <c r="AC4" s="41">
+      <c r="W4" s="46"/>
+      <c r="X4" s="46"/>
+      <c r="Y4" s="46"/>
+      <c r="Z4" s="46"/>
+      <c r="AA4" s="46"/>
+      <c r="AB4" s="47"/>
+      <c r="AC4" s="45">
         <f>AC5</f>
         <v>44865</v>
       </c>
-      <c r="AD4" s="42"/>
-      <c r="AE4" s="42"/>
-      <c r="AF4" s="42"/>
-      <c r="AG4" s="42"/>
-      <c r="AH4" s="42"/>
-      <c r="AI4" s="43"/>
-      <c r="AJ4" s="41">
+      <c r="AD4" s="46"/>
+      <c r="AE4" s="46"/>
+      <c r="AF4" s="46"/>
+      <c r="AG4" s="46"/>
+      <c r="AH4" s="46"/>
+      <c r="AI4" s="47"/>
+      <c r="AJ4" s="45">
         <f>AJ5</f>
         <v>44872</v>
       </c>
-      <c r="AK4" s="42"/>
-      <c r="AL4" s="42"/>
-      <c r="AM4" s="42"/>
-      <c r="AN4" s="42"/>
-      <c r="AO4" s="42"/>
-      <c r="AP4" s="43"/>
-      <c r="AQ4" s="41">
+      <c r="AK4" s="46"/>
+      <c r="AL4" s="46"/>
+      <c r="AM4" s="46"/>
+      <c r="AN4" s="46"/>
+      <c r="AO4" s="46"/>
+      <c r="AP4" s="47"/>
+      <c r="AQ4" s="45">
         <f>AQ5</f>
         <v>44879</v>
       </c>
-      <c r="AR4" s="42"/>
-      <c r="AS4" s="42"/>
-      <c r="AT4" s="42"/>
-      <c r="AU4" s="42"/>
-      <c r="AV4" s="42"/>
-      <c r="AW4" s="43"/>
-      <c r="AX4" s="41">
+      <c r="AR4" s="46"/>
+      <c r="AS4" s="46"/>
+      <c r="AT4" s="46"/>
+      <c r="AU4" s="46"/>
+      <c r="AV4" s="46"/>
+      <c r="AW4" s="47"/>
+      <c r="AX4" s="45">
         <f>AX5</f>
         <v>44886</v>
       </c>
-      <c r="AY4" s="42"/>
-      <c r="AZ4" s="42"/>
-      <c r="BA4" s="42"/>
-      <c r="BB4" s="42"/>
-      <c r="BC4" s="42"/>
-      <c r="BD4" s="43"/>
-      <c r="BE4" s="41">
+      <c r="AY4" s="46"/>
+      <c r="AZ4" s="46"/>
+      <c r="BA4" s="46"/>
+      <c r="BB4" s="46"/>
+      <c r="BC4" s="46"/>
+      <c r="BD4" s="47"/>
+      <c r="BE4" s="45">
         <f>BE5</f>
         <v>44893</v>
       </c>
-      <c r="BF4" s="42"/>
-      <c r="BG4" s="42"/>
-      <c r="BH4" s="42"/>
-      <c r="BI4" s="42"/>
-      <c r="BJ4" s="42"/>
-      <c r="BK4" s="43"/>
-      <c r="BL4" s="41">
+      <c r="BF4" s="46"/>
+      <c r="BG4" s="46"/>
+      <c r="BH4" s="46"/>
+      <c r="BI4" s="46"/>
+      <c r="BJ4" s="46"/>
+      <c r="BK4" s="47"/>
+      <c r="BL4" s="45">
         <f>BL5</f>
         <v>44900</v>
       </c>
-      <c r="BM4" s="42"/>
-      <c r="BN4" s="42"/>
-      <c r="BO4" s="42"/>
-      <c r="BP4" s="42"/>
-      <c r="BQ4" s="42"/>
-      <c r="BR4" s="43"/>
-      <c r="BS4" s="41">
+      <c r="BM4" s="46"/>
+      <c r="BN4" s="46"/>
+      <c r="BO4" s="46"/>
+      <c r="BP4" s="46"/>
+      <c r="BQ4" s="46"/>
+      <c r="BR4" s="47"/>
+      <c r="BS4" s="45">
         <f>BS5</f>
         <v>44907</v>
       </c>
-      <c r="BT4" s="42"/>
-      <c r="BU4" s="42"/>
-      <c r="BV4" s="42"/>
-      <c r="BW4" s="42"/>
-      <c r="BX4" s="42"/>
-      <c r="BY4" s="43"/>
-      <c r="BZ4" s="41">
+      <c r="BT4" s="46"/>
+      <c r="BU4" s="46"/>
+      <c r="BV4" s="46"/>
+      <c r="BW4" s="46"/>
+      <c r="BX4" s="46"/>
+      <c r="BY4" s="47"/>
+      <c r="BZ4" s="45">
         <f>BZ5</f>
         <v>44914</v>
       </c>
-      <c r="CA4" s="42"/>
-      <c r="CB4" s="42"/>
-      <c r="CC4" s="42"/>
-      <c r="CD4" s="42"/>
-      <c r="CE4" s="42"/>
-      <c r="CF4" s="43"/>
-      <c r="CG4" s="41">
+      <c r="CA4" s="46"/>
+      <c r="CB4" s="46"/>
+      <c r="CC4" s="46"/>
+      <c r="CD4" s="46"/>
+      <c r="CE4" s="46"/>
+      <c r="CF4" s="47"/>
+      <c r="CG4" s="45">
         <f>CG5</f>
         <v>44921</v>
       </c>
-      <c r="CH4" s="42"/>
-      <c r="CI4" s="42"/>
-      <c r="CJ4" s="42"/>
-      <c r="CK4" s="42"/>
-      <c r="CL4" s="42"/>
-      <c r="CM4" s="43"/>
-      <c r="CN4" s="41">
+      <c r="CH4" s="46"/>
+      <c r="CI4" s="46"/>
+      <c r="CJ4" s="46"/>
+      <c r="CK4" s="46"/>
+      <c r="CL4" s="46"/>
+      <c r="CM4" s="47"/>
+      <c r="CN4" s="45">
         <f>CN5</f>
         <v>44928</v>
       </c>
-      <c r="CO4" s="42"/>
-      <c r="CP4" s="42"/>
-      <c r="CQ4" s="42"/>
-      <c r="CR4" s="42"/>
-      <c r="CS4" s="42"/>
-      <c r="CT4" s="43"/>
-      <c r="CU4" s="41">
+      <c r="CO4" s="46"/>
+      <c r="CP4" s="46"/>
+      <c r="CQ4" s="46"/>
+      <c r="CR4" s="46"/>
+      <c r="CS4" s="46"/>
+      <c r="CT4" s="47"/>
+      <c r="CU4" s="45">
         <f>CU5</f>
         <v>44935</v>
       </c>
-      <c r="CV4" s="42"/>
-      <c r="CW4" s="42"/>
-      <c r="CX4" s="42"/>
-      <c r="CY4" s="42"/>
-      <c r="CZ4" s="42"/>
-      <c r="DA4" s="43"/>
-      <c r="DB4" s="41">
+      <c r="CV4" s="46"/>
+      <c r="CW4" s="46"/>
+      <c r="CX4" s="46"/>
+      <c r="CY4" s="46"/>
+      <c r="CZ4" s="46"/>
+      <c r="DA4" s="47"/>
+      <c r="DB4" s="45">
         <f>DB5</f>
         <v>44942</v>
       </c>
-      <c r="DC4" s="42"/>
-      <c r="DD4" s="42"/>
-      <c r="DE4" s="42"/>
-      <c r="DF4" s="42"/>
-      <c r="DG4" s="42"/>
-      <c r="DH4" s="43"/>
-      <c r="DI4" s="41">
+      <c r="DC4" s="46"/>
+      <c r="DD4" s="46"/>
+      <c r="DE4" s="46"/>
+      <c r="DF4" s="46"/>
+      <c r="DG4" s="46"/>
+      <c r="DH4" s="47"/>
+      <c r="DI4" s="45">
         <f>DI5</f>
         <v>44949</v>
       </c>
-      <c r="DJ4" s="42"/>
-      <c r="DK4" s="42"/>
-      <c r="DL4" s="42"/>
-      <c r="DM4" s="42"/>
-      <c r="DN4" s="42"/>
-      <c r="DO4" s="43"/>
-      <c r="DP4" s="41">
+      <c r="DJ4" s="46"/>
+      <c r="DK4" s="46"/>
+      <c r="DL4" s="46"/>
+      <c r="DM4" s="46"/>
+      <c r="DN4" s="46"/>
+      <c r="DO4" s="47"/>
+      <c r="DP4" s="45">
         <f>DP5</f>
         <v>44956</v>
       </c>
-      <c r="DQ4" s="42"/>
-      <c r="DR4" s="42"/>
-      <c r="DS4" s="42"/>
-      <c r="DT4" s="42"/>
-      <c r="DU4" s="42"/>
-      <c r="DV4" s="43"/>
-      <c r="DW4" s="41">
+      <c r="DQ4" s="46"/>
+      <c r="DR4" s="46"/>
+      <c r="DS4" s="46"/>
+      <c r="DT4" s="46"/>
+      <c r="DU4" s="46"/>
+      <c r="DV4" s="47"/>
+      <c r="DW4" s="45">
         <f>DW5</f>
         <v>44963</v>
       </c>
-      <c r="DX4" s="42"/>
-      <c r="DY4" s="42"/>
-      <c r="DZ4" s="42"/>
-      <c r="EA4" s="42"/>
-      <c r="EB4" s="42"/>
-      <c r="EC4" s="43"/>
-      <c r="ED4" s="41">
+      <c r="DX4" s="46"/>
+      <c r="DY4" s="46"/>
+      <c r="DZ4" s="46"/>
+      <c r="EA4" s="46"/>
+      <c r="EB4" s="46"/>
+      <c r="EC4" s="47"/>
+      <c r="ED4" s="45">
         <f>ED5</f>
         <v>44970</v>
       </c>
-      <c r="EE4" s="42"/>
-      <c r="EF4" s="42"/>
-      <c r="EG4" s="42"/>
-      <c r="EH4" s="42"/>
-      <c r="EI4" s="42"/>
-      <c r="EJ4" s="43"/>
-      <c r="EK4" s="41">
+      <c r="EE4" s="46"/>
+      <c r="EF4" s="46"/>
+      <c r="EG4" s="46"/>
+      <c r="EH4" s="46"/>
+      <c r="EI4" s="46"/>
+      <c r="EJ4" s="47"/>
+      <c r="EK4" s="45">
         <f>EK5</f>
         <v>44977</v>
       </c>
-      <c r="EL4" s="42"/>
-      <c r="EM4" s="42"/>
-      <c r="EN4" s="42"/>
-      <c r="EO4" s="42"/>
-      <c r="EP4" s="42"/>
-      <c r="EQ4" s="43"/>
-      <c r="ER4" s="41">
+      <c r="EL4" s="46"/>
+      <c r="EM4" s="46"/>
+      <c r="EN4" s="46"/>
+      <c r="EO4" s="46"/>
+      <c r="EP4" s="46"/>
+      <c r="EQ4" s="47"/>
+      <c r="ER4" s="45">
         <f>ER5</f>
         <v>44984</v>
       </c>
-      <c r="ES4" s="42"/>
-      <c r="ET4" s="42"/>
-      <c r="EU4" s="42"/>
-      <c r="EV4" s="42"/>
-      <c r="EW4" s="42"/>
-      <c r="EX4" s="43"/>
-      <c r="EY4" s="41">
+      <c r="ES4" s="46"/>
+      <c r="ET4" s="46"/>
+      <c r="EU4" s="46"/>
+      <c r="EV4" s="46"/>
+      <c r="EW4" s="46"/>
+      <c r="EX4" s="47"/>
+      <c r="EY4" s="45">
         <f>EY5</f>
         <v>44991</v>
       </c>
-      <c r="EZ4" s="42"/>
-      <c r="FA4" s="42"/>
-      <c r="FB4" s="42"/>
-      <c r="FC4" s="42"/>
-      <c r="FD4" s="42"/>
-      <c r="FE4" s="43"/>
-      <c r="FF4" s="41">
+      <c r="EZ4" s="46"/>
+      <c r="FA4" s="46"/>
+      <c r="FB4" s="46"/>
+      <c r="FC4" s="46"/>
+      <c r="FD4" s="46"/>
+      <c r="FE4" s="47"/>
+      <c r="FF4" s="45">
         <f>FF5</f>
         <v>44998</v>
       </c>
-      <c r="FG4" s="42"/>
-      <c r="FH4" s="42"/>
-      <c r="FI4" s="42"/>
-      <c r="FJ4" s="42"/>
-      <c r="FK4" s="42"/>
-      <c r="FL4" s="43"/>
-      <c r="FM4" s="41">
+      <c r="FG4" s="46"/>
+      <c r="FH4" s="46"/>
+      <c r="FI4" s="46"/>
+      <c r="FJ4" s="46"/>
+      <c r="FK4" s="46"/>
+      <c r="FL4" s="47"/>
+      <c r="FM4" s="45">
         <f>FM5</f>
         <v>45005</v>
       </c>
-      <c r="FN4" s="42"/>
-      <c r="FO4" s="42"/>
-      <c r="FP4" s="42"/>
-      <c r="FQ4" s="42"/>
-      <c r="FR4" s="42"/>
-      <c r="FS4" s="43"/>
-      <c r="FT4" s="41">
+      <c r="FN4" s="46"/>
+      <c r="FO4" s="46"/>
+      <c r="FP4" s="46"/>
+      <c r="FQ4" s="46"/>
+      <c r="FR4" s="46"/>
+      <c r="FS4" s="47"/>
+      <c r="FT4" s="45">
         <f>FT5</f>
         <v>45012</v>
       </c>
-      <c r="FU4" s="42"/>
-      <c r="FV4" s="42"/>
-      <c r="FW4" s="42"/>
-      <c r="FX4" s="42"/>
-      <c r="FY4" s="42"/>
-      <c r="FZ4" s="43"/>
-      <c r="GA4" s="41">
+      <c r="FU4" s="46"/>
+      <c r="FV4" s="46"/>
+      <c r="FW4" s="46"/>
+      <c r="FX4" s="46"/>
+      <c r="FY4" s="46"/>
+      <c r="FZ4" s="47"/>
+      <c r="GA4" s="45">
         <f>GA5</f>
         <v>45019</v>
       </c>
-      <c r="GB4" s="42"/>
-      <c r="GC4" s="42"/>
-      <c r="GD4" s="42"/>
-      <c r="GE4" s="42"/>
-      <c r="GF4" s="42"/>
-      <c r="GG4" s="43"/>
-      <c r="GH4" s="41">
+      <c r="GB4" s="46"/>
+      <c r="GC4" s="46"/>
+      <c r="GD4" s="46"/>
+      <c r="GE4" s="46"/>
+      <c r="GF4" s="46"/>
+      <c r="GG4" s="47"/>
+      <c r="GH4" s="45">
         <f>GH5</f>
         <v>45026</v>
       </c>
-      <c r="GI4" s="42"/>
-      <c r="GJ4" s="42"/>
-      <c r="GK4" s="42"/>
-      <c r="GL4" s="42"/>
-      <c r="GM4" s="42"/>
-      <c r="GN4" s="43"/>
-      <c r="GO4" s="41">
+      <c r="GI4" s="46"/>
+      <c r="GJ4" s="46"/>
+      <c r="GK4" s="46"/>
+      <c r="GL4" s="46"/>
+      <c r="GM4" s="46"/>
+      <c r="GN4" s="47"/>
+      <c r="GO4" s="45">
         <f>GO5</f>
         <v>45033</v>
       </c>
-      <c r="GP4" s="42"/>
-      <c r="GQ4" s="42"/>
-      <c r="GR4" s="42"/>
-      <c r="GS4" s="42"/>
-      <c r="GT4" s="42"/>
-      <c r="GU4" s="43"/>
+      <c r="GP4" s="46"/>
+      <c r="GQ4" s="46"/>
+      <c r="GR4" s="46"/>
+      <c r="GS4" s="46"/>
+      <c r="GT4" s="46"/>
+      <c r="GU4" s="47"/>
     </row>
     <row r="5" spans="1:203" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
@@ -3678,7 +3678,7 @@
       <c r="A8" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="41" t="s">
         <v>78</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -3695,38 +3695,38 @@
         <f t="shared" ref="G8:G49" si="16">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>32</v>
       </c>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="46"/>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="46"/>
-      <c r="S8" s="46"/>
-      <c r="T8" s="46"/>
-      <c r="U8" s="46"/>
-      <c r="V8" s="46"/>
-      <c r="W8" s="46"/>
-      <c r="X8" s="46"/>
-      <c r="Y8" s="46"/>
-      <c r="Z8" s="46"/>
-      <c r="AA8" s="46"/>
-      <c r="AB8" s="46"/>
-      <c r="AC8" s="46"/>
-      <c r="AD8" s="46"/>
-      <c r="AE8" s="46"/>
-      <c r="AF8" s="46"/>
-      <c r="AG8" s="46"/>
-      <c r="AH8" s="46"/>
-      <c r="AI8" s="46"/>
-      <c r="AJ8" s="46"/>
-      <c r="AK8" s="46"/>
-      <c r="AL8" s="46"/>
-      <c r="AM8" s="46"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="42"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="42"/>
+      <c r="T8" s="42"/>
+      <c r="U8" s="42"/>
+      <c r="V8" s="42"/>
+      <c r="W8" s="42"/>
+      <c r="X8" s="42"/>
+      <c r="Y8" s="42"/>
+      <c r="Z8" s="42"/>
+      <c r="AA8" s="42"/>
+      <c r="AB8" s="42"/>
+      <c r="AC8" s="42"/>
+      <c r="AD8" s="42"/>
+      <c r="AE8" s="42"/>
+      <c r="AF8" s="42"/>
+      <c r="AG8" s="42"/>
+      <c r="AH8" s="42"/>
+      <c r="AI8" s="42"/>
+      <c r="AJ8" s="42"/>
+      <c r="AK8" s="42"/>
+      <c r="AL8" s="42"/>
+      <c r="AM8" s="42"/>
       <c r="AN8" s="13"/>
       <c r="AO8" s="13"/>
       <c r="AP8" s="13"/>
@@ -3893,10 +3893,10 @@
       <c r="GU8" s="13"/>
     </row>
     <row r="9" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="41" t="s">
         <v>72</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -4112,7 +4112,7 @@
     </row>
     <row r="10" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="26"/>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="41" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -4328,7 +4328,7 @@
     </row>
     <row r="11" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="26"/>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="44" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -4544,7 +4544,7 @@
     </row>
     <row r="12" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="27"/>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="44" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -4760,7 +4760,7 @@
     </row>
     <row r="13" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="26"/>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="41" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -4976,7 +4976,7 @@
     </row>
     <row r="14" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="26"/>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="44" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -5192,7 +5192,7 @@
     </row>
     <row r="15" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="26"/>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="41" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -5408,7 +5408,7 @@
     </row>
     <row r="16" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="26"/>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="44" t="s">
         <v>40</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -5624,7 +5624,7 @@
     </row>
     <row r="17" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="26"/>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="44" t="s">
         <v>41</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -5840,7 +5840,7 @@
     </row>
     <row r="18" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="26"/>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="44" t="s">
         <v>42</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -6056,7 +6056,7 @@
     </row>
     <row r="19" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="26"/>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="44" t="s">
         <v>43</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -6272,7 +6272,7 @@
     </row>
     <row r="20" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="26"/>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="41" t="s">
         <v>44</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -6488,7 +6488,7 @@
     </row>
     <row r="21" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="26"/>
-      <c r="B21" s="48" t="s">
+      <c r="B21" s="41" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -6704,7 +6704,7 @@
     </row>
     <row r="22" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="26"/>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="41" t="s">
         <v>46</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -6920,7 +6920,7 @@
     </row>
     <row r="23" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="26"/>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="44" t="s">
         <v>47</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -7136,7 +7136,7 @@
     </row>
     <row r="24" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="26"/>
-      <c r="B24" s="48" t="s">
+      <c r="B24" s="44" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -7352,7 +7352,7 @@
     </row>
     <row r="25" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="26"/>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="41" t="s">
         <v>49</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -7568,7 +7568,7 @@
     </row>
     <row r="26" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="26"/>
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="41" t="s">
         <v>60</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -7781,7 +7781,7 @@
     </row>
     <row r="27" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="26"/>
-      <c r="B27" s="48" t="s">
+      <c r="B27" s="41" t="s">
         <v>73</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -12702,26 +12702,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="FM4:FS4"/>
-    <mergeCell ref="FT4:FZ4"/>
-    <mergeCell ref="GA4:GG4"/>
-    <mergeCell ref="GH4:GN4"/>
-    <mergeCell ref="GO4:GU4"/>
-    <mergeCell ref="ED4:EJ4"/>
-    <mergeCell ref="EK4:EQ4"/>
-    <mergeCell ref="ER4:EX4"/>
-    <mergeCell ref="EY4:FE4"/>
-    <mergeCell ref="FF4:FL4"/>
-    <mergeCell ref="CU4:DA4"/>
-    <mergeCell ref="DB4:DH4"/>
-    <mergeCell ref="DI4:DO4"/>
-    <mergeCell ref="DP4:DV4"/>
-    <mergeCell ref="DW4:EC4"/>
-    <mergeCell ref="BL4:BR4"/>
-    <mergeCell ref="BS4:BY4"/>
-    <mergeCell ref="BZ4:CF4"/>
-    <mergeCell ref="CG4:CM4"/>
-    <mergeCell ref="CN4:CT4"/>
     <mergeCell ref="BE4:BK4"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="H4:N4"/>
@@ -12731,6 +12711,26 @@
     <mergeCell ref="AJ4:AP4"/>
     <mergeCell ref="AQ4:AW4"/>
     <mergeCell ref="AX4:BD4"/>
+    <mergeCell ref="BL4:BR4"/>
+    <mergeCell ref="BS4:BY4"/>
+    <mergeCell ref="BZ4:CF4"/>
+    <mergeCell ref="CG4:CM4"/>
+    <mergeCell ref="CN4:CT4"/>
+    <mergeCell ref="CU4:DA4"/>
+    <mergeCell ref="DB4:DH4"/>
+    <mergeCell ref="DI4:DO4"/>
+    <mergeCell ref="DP4:DV4"/>
+    <mergeCell ref="DW4:EC4"/>
+    <mergeCell ref="ED4:EJ4"/>
+    <mergeCell ref="EK4:EQ4"/>
+    <mergeCell ref="ER4:EX4"/>
+    <mergeCell ref="EY4:FE4"/>
+    <mergeCell ref="FF4:FL4"/>
+    <mergeCell ref="FM4:FS4"/>
+    <mergeCell ref="FT4:FZ4"/>
+    <mergeCell ref="GA4:GG4"/>
+    <mergeCell ref="GH4:GN4"/>
+    <mergeCell ref="GO4:GU4"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:GU40 H44:GU49">
     <cfRule type="expression" dxfId="11" priority="54">

</xml_diff>

<commit_message>
Updated login page GUI. Created the employee details frame with notes, schedule and time cards. Created the notes frame to be functional.
</commit_message>
<xml_diff>
--- a/Development Timelines/GanttChart_Iteration3.xlsx
+++ b/Development Timelines/GanttChart_Iteration3.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D854EC64-6BFE-4C11-94FA-0606570DF73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B9400B-48CE-4046-A954-30A3B0EB34F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1445,9 +1445,9 @@
   </sheetPr>
   <dimension ref="A1:GU49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="81" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4976,7 +4976,7 @@
     </row>
     <row r="14" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="26"/>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="41" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -5408,7 +5408,7 @@
     </row>
     <row r="16" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="26"/>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="41" t="s">
         <v>40</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -6272,7 +6272,7 @@
     </row>
     <row r="20" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="26"/>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="41" t="s">
         <v>44</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -6704,7 +6704,7 @@
     </row>
     <row r="22" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="26"/>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="41" t="s">
         <v>46</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -12702,26 +12702,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="FM4:FS4"/>
-    <mergeCell ref="FT4:FZ4"/>
-    <mergeCell ref="GA4:GG4"/>
-    <mergeCell ref="GH4:GN4"/>
-    <mergeCell ref="GO4:GU4"/>
-    <mergeCell ref="ED4:EJ4"/>
-    <mergeCell ref="EK4:EQ4"/>
-    <mergeCell ref="ER4:EX4"/>
-    <mergeCell ref="EY4:FE4"/>
-    <mergeCell ref="FF4:FL4"/>
-    <mergeCell ref="CU4:DA4"/>
-    <mergeCell ref="DB4:DH4"/>
-    <mergeCell ref="DI4:DO4"/>
-    <mergeCell ref="DP4:DV4"/>
-    <mergeCell ref="DW4:EC4"/>
-    <mergeCell ref="BL4:BR4"/>
-    <mergeCell ref="BS4:BY4"/>
-    <mergeCell ref="BZ4:CF4"/>
-    <mergeCell ref="CG4:CM4"/>
-    <mergeCell ref="CN4:CT4"/>
     <mergeCell ref="BE4:BK4"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="H4:N4"/>
@@ -12731,6 +12711,26 @@
     <mergeCell ref="AJ4:AP4"/>
     <mergeCell ref="AQ4:AW4"/>
     <mergeCell ref="AX4:BD4"/>
+    <mergeCell ref="BL4:BR4"/>
+    <mergeCell ref="BS4:BY4"/>
+    <mergeCell ref="BZ4:CF4"/>
+    <mergeCell ref="CG4:CM4"/>
+    <mergeCell ref="CN4:CT4"/>
+    <mergeCell ref="CU4:DA4"/>
+    <mergeCell ref="DB4:DH4"/>
+    <mergeCell ref="DI4:DO4"/>
+    <mergeCell ref="DP4:DV4"/>
+    <mergeCell ref="DW4:EC4"/>
+    <mergeCell ref="ED4:EJ4"/>
+    <mergeCell ref="EK4:EQ4"/>
+    <mergeCell ref="ER4:EX4"/>
+    <mergeCell ref="EY4:FE4"/>
+    <mergeCell ref="FF4:FL4"/>
+    <mergeCell ref="FM4:FS4"/>
+    <mergeCell ref="FT4:FZ4"/>
+    <mergeCell ref="GA4:GG4"/>
+    <mergeCell ref="GH4:GN4"/>
+    <mergeCell ref="GO4:GU4"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:GU40 H44:GU49">
     <cfRule type="expression" dxfId="11" priority="54">

</xml_diff>